<commit_message>
changed excel sheet settings
</commit_message>
<xml_diff>
--- a/graphs/common_feature_analysis.xlsx
+++ b/graphs/common_feature_analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="166">
   <si>
     <t>Feature</t>
   </si>
@@ -30,172 +30,490 @@
     <t>Lasso_</t>
   </si>
   <si>
+    <t>B2a_0g</t>
+  </si>
+  <si>
+    <t>lrig_0_cd</t>
+  </si>
+  <si>
+    <t>primsev_cocaine</t>
+  </si>
+  <si>
+    <t>primsev_other</t>
+  </si>
+  <si>
+    <t>primsev_alcohol</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>dssg_0_cd</t>
+  </si>
+  <si>
     <t>r4ag_0_cd</t>
   </si>
   <si>
+    <t>%_povertyg</t>
+  </si>
+  <si>
+    <t>PYS9Sxg_cd</t>
+  </si>
+  <si>
+    <t>epsg_0_cd</t>
+  </si>
+  <si>
     <t>nonwhite</t>
   </si>
   <si>
+    <t>primsev_amphetamines</t>
+  </si>
+  <si>
+    <t>SESg_0_cd</t>
+  </si>
+  <si>
+    <t>pop_deng</t>
+  </si>
+  <si>
+    <t>murder_numg</t>
+  </si>
+  <si>
+    <t>primsev_opioids</t>
+  </si>
+  <si>
+    <t>adhdg_0_cd</t>
+  </si>
+  <si>
+    <t>gvsg_cd</t>
+  </si>
+  <si>
+    <t>prsatx_cd</t>
+  </si>
+  <si>
+    <t>unemplmt_cd</t>
+  </si>
+  <si>
+    <t>cjsig_0_cd</t>
+  </si>
+  <si>
+    <t>srig_0_cd</t>
+  </si>
+  <si>
+    <t>CWSg_0_cd</t>
+  </si>
+  <si>
+    <t>homeless_0_cd</t>
+  </si>
+  <si>
+    <t>cdsg_0_cd</t>
+  </si>
+  <si>
+    <t>primsev_marijuana</t>
+  </si>
+  <si>
     <t>ncar_cd</t>
   </si>
   <si>
-    <t>B2a_0g</t>
-  </si>
-  <si>
-    <t>pop_deng</t>
-  </si>
-  <si>
-    <t>primsev_opioids</t>
-  </si>
-  <si>
-    <t>PYS9Sxg_cd</t>
-  </si>
-  <si>
-    <t>primsev_other</t>
-  </si>
-  <si>
-    <t>srig_0_cd</t>
-  </si>
-  <si>
-    <t>%_povertyg</t>
-  </si>
-  <si>
-    <t>cjsig_0_cd</t>
-  </si>
-  <si>
-    <t>murder_numg</t>
-  </si>
-  <si>
-    <t>dssg_0_cd</t>
+    <t>TRIg_0_cd</t>
+  </si>
+  <si>
+    <t>('B2a_0g_0', 0.9412357823218712)</t>
+  </si>
+  <si>
+    <t>('lrig_0_cd_0', 0.9977892237691484)</t>
+  </si>
+  <si>
+    <t>('primsev_cocaine', 1.0179736684060987)</t>
+  </si>
+  <si>
+    <t>('primsev_other', 1.0014911750546007)</t>
+  </si>
+  <si>
+    <t>('primsev_alcohol', 0.987338482392838)</t>
+  </si>
+  <si>
+    <t>('female', 1.0002922034547932)</t>
+  </si>
+  <si>
+    <t>('dssg_0_cd_0', 0.9441341914929483)</t>
+  </si>
+  <si>
+    <t>('r4ag_0_cd_0', 0.9946156235050998)</t>
+  </si>
+  <si>
+    <t>('%_povertyg_0', 0.9428459229572359)</t>
+  </si>
+  <si>
+    <t>('PYS9Sxg_cd_0', 0.9879839962248869)</t>
+  </si>
+  <si>
+    <t>('epsg_0_cd_0', 1.007377978538842)</t>
+  </si>
+  <si>
+    <t>('nonwhite', 0.9200349429378138)</t>
+  </si>
+  <si>
+    <t>('primsev_amphetamines', 0.944771776282438)</t>
+  </si>
+  <si>
+    <t>('SESg_0_cd_0', 0.995504554903149)</t>
+  </si>
+  <si>
+    <t>('pop_deng_0', 0.0)</t>
+  </si>
+  <si>
+    <t>('murder_numg_0', 1.4391733054685725)</t>
+  </si>
+  <si>
+    <t>('primsev_opioids', 1.026428458348139)</t>
+  </si>
+  <si>
+    <t>('adhdg_0_cd_0', 0.9994294807189732)</t>
+  </si>
+  <si>
+    <t>('gvsg_cd_0', 0.9566823627609788)</t>
+  </si>
+  <si>
+    <t>('prsatx_cd_0', 1.000255464342523)</t>
+  </si>
+  <si>
+    <t>('unemplmt_cd', 0.9922395728915905)</t>
+  </si>
+  <si>
+    <t>('cjsig_0_cd_0', 0.9208582510771413)</t>
+  </si>
+  <si>
+    <t>('srig_0_cd_0', 0.9994028046273031)</t>
+  </si>
+  <si>
+    <t>('CWSg_0_cd_0', 0.9992729119011987)</t>
+  </si>
+  <si>
+    <t>('homeless_0_cd_0', 1.003953393254234)</t>
+  </si>
+  <si>
+    <t>('cdsg_0_cd_0', 0.9975251447420269)</t>
+  </si>
+  <si>
+    <t>('primsev_marijuana', 0.9997125598888561)</t>
+  </si>
+  <si>
+    <t>('ncar_cd_0', 1.0682566904441027)</t>
+  </si>
+  <si>
+    <t>('TRIg_0_cd_0', 0.999951925545857)</t>
+  </si>
+  <si>
+    <t>('B2a_0g_2', 1.128348158691236)</t>
+  </si>
+  <si>
+    <t>('lrig_0_cd_2', 0.9973214039209904)</t>
+  </si>
+  <si>
+    <t>('dssg_0_cd_2', 1.0000551990385265)</t>
   </si>
   <si>
     <t>('r4ag_0_cd_2', 1.1779218746872526)</t>
   </si>
   <si>
-    <t>('nonwhite', 0.9200349429378138)</t>
-  </si>
-  <si>
-    <t>('ncar_cd_0', 1.0682566904441027)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_2', 1.128348158691236)</t>
-  </si>
-  <si>
-    <t>('pop_deng_0', 0.0)</t>
-  </si>
-  <si>
-    <t>('primsev_opioids', 0.0)</t>
-  </si>
-  <si>
-    <t>('PYS9Sxg_cd_0', 0.0)</t>
-  </si>
-  <si>
-    <t>('primsev_other', 0.0)</t>
-  </si>
-  <si>
-    <t>('srig_0_cd_2', 0.0)</t>
-  </si>
-  <si>
-    <t>('%_povertyg_0', 0.9428459229572359)</t>
-  </si>
-  <si>
-    <t>('cjsig_0_cd_0', 0.9208582510771413)</t>
-  </si>
-  <si>
-    <t>('murder_numg_0', 1.4391733054685725)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_0', 0.9441341914929483)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_0', 0.0)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_0', 0.9412357823218712)</t>
+    <t>('PYS9Sxg_cd_2', 0.0)</t>
+  </si>
+  <si>
+    <t>('epsg_0_cd_2', 0.9999470231363313)</t>
+  </si>
+  <si>
+    <t>('SESg_0_cd_2', 0.9830581368257205)</t>
+  </si>
+  <si>
+    <t>('pop_deng_2', 0.0)</t>
+  </si>
+  <si>
+    <t>('murder_numg_2', 1.003401526386335)</t>
+  </si>
+  <si>
+    <t>('adhdg_0_cd_2', 1.0052338567367003)</t>
+  </si>
+  <si>
+    <t>('gvsg_cd_2', 1.0041789625594866)</t>
   </si>
   <si>
     <t>('cjsig_0_cd_2', 1.074330210753723)</t>
   </si>
   <si>
-    <t>('murder_numg_2', 0.0)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_2', 0.0)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_2', 0.0)</t>
+    <t>('srig_0_cd_2', 0.9998494995714677)</t>
+  </si>
+  <si>
+    <t>('CWSg_0_cd_2', 0.0)</t>
+  </si>
+  <si>
+    <t>('cdsg_0_cd_2', 0.0)</t>
+  </si>
+  <si>
+    <t>('TRIg_0_cd_2', 0.9878892609049318)</t>
+  </si>
+  <si>
+    <t>('B2a_0g_0', 0.9827316912641159)</t>
+  </si>
+  <si>
+    <t>('lrig_0_cd_0', 0.9772117616051937)</t>
+  </si>
+  <si>
+    <t>('primsev_cocaine', 1.026355968573712)</t>
+  </si>
+  <si>
+    <t>('primsev_other', 1.0497040679188336)</t>
+  </si>
+  <si>
+    <t>('primsev_alcohol', 0.957609263934147)</t>
+  </si>
+  <si>
+    <t>('female', 0.9937523800149287)</t>
+  </si>
+  <si>
+    <t>('dssg_0_cd_0', 1.000114003069927)</t>
+  </si>
+  <si>
+    <t>('r4ag_0_cd_0', 0.8946958002258929)</t>
+  </si>
+  <si>
+    <t>('%_povertyg_0', 0.9739665008654048)</t>
+  </si>
+  <si>
+    <t>('PYS9Sxg_cd_0', 0.9353836116963504)</t>
+  </si>
+  <si>
+    <t>('epsg_0_cd_0', 0.9969418452634656)</t>
   </si>
   <si>
     <t>('nonwhite', 0.9189422138816976)</t>
   </si>
   <si>
-    <t>('ncar_cd_0', 0.0)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_2', 0.0)</t>
+    <t>('primsev_amphetamines', 0.9838176681964953)</t>
+  </si>
+  <si>
+    <t>('SESg_0_cd_0', 0.997424526647715)</t>
   </si>
   <si>
     <t>('pop_deng_0', 1.0546216678905302)</t>
   </si>
   <si>
-    <t>('PYS9Sxg_cd_0', 0.9353836116963504)</t>
-  </si>
-  <si>
-    <t>('primsev_other', 1.0497040679188336)</t>
-  </si>
-  <si>
-    <t>('%_povertyg_0', 0.0)</t>
+    <t>('murder_numg_0', 0.0)</t>
+  </si>
+  <si>
+    <t>('primsev_opioids', 1.001360177902959)</t>
+  </si>
+  <si>
+    <t>('adhdg_0_cd_0', 1.0001743918236392)</t>
+  </si>
+  <si>
+    <t>('gvsg_cd_0', 0.9952267711981352)</t>
+  </si>
+  <si>
+    <t>('prsatx_cd_0', 0.9411367306303198)</t>
+  </si>
+  <si>
+    <t>('unemplmt_cd', 0.9952859575926934)</t>
   </si>
   <si>
     <t>('cjsig_0_cd_0', 0.9354206641997593)</t>
   </si>
   <si>
-    <t>('murder_numg_0', 0.0)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_0', 0.0)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_0', 0.8946958002258929)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_0', 0.0)</t>
-  </si>
-  <si>
-    <t>('cjsig_0_cd_2', 0.0)</t>
+    <t>('srig_0_cd_0', 0.9985401922503998)</t>
+  </si>
+  <si>
+    <t>('CWSg_0_cd_0', 1.0041140618481026)</t>
+  </si>
+  <si>
+    <t>('homeless_0_cd_0', 1.0021357370718738)</t>
+  </si>
+  <si>
+    <t>('cdsg_0_cd_0', 0.9468888416799393)</t>
+  </si>
+  <si>
+    <t>('primsev_marijuana', 0.9998460155514156)</t>
+  </si>
+  <si>
+    <t>('ncar_cd_0', 1.0074496367042836)</t>
+  </si>
+  <si>
+    <t>('TRIg_0_cd_0', 1.0242608134558155)</t>
+  </si>
+  <si>
+    <t>('B2a_0g_2', 0.9763382997222922)</t>
+  </si>
+  <si>
+    <t>('lrig_0_cd_2', 1.0030057032567987)</t>
+  </si>
+  <si>
+    <t>('dssg_0_cd_2', 0.9876473847842663)</t>
+  </si>
+  <si>
+    <t>('r4ag_0_cd_2', 0.9974870090150953)</t>
+  </si>
+  <si>
+    <t>('epsg_0_cd_2', 1.0423813392017787)</t>
+  </si>
+  <si>
+    <t>('SESg_0_cd_2', 0.9897939071604813)</t>
   </si>
   <si>
     <t>('murder_numg_2', 0.9575506176558319)</t>
   </si>
   <si>
-    <t>('nonwhite', 0.0)</t>
+    <t>('adhdg_0_cd_2', 0.9997572102938117)</t>
+  </si>
+  <si>
+    <t>('gvsg_cd_2', 0.9910236335438817)</t>
+  </si>
+  <si>
+    <t>('cjsig_0_cd_2', 0.9986804452510393)</t>
+  </si>
+  <si>
+    <t>('srig_0_cd_2', 1.0183149928931163)</t>
+  </si>
+  <si>
+    <t>('CWSg_0_cd_2', 1.0025903321333538)</t>
+  </si>
+  <si>
+    <t>('cdsg_0_cd_2', 0.9999997889576135)</t>
+  </si>
+  <si>
+    <t>('TRIg_0_cd_2', 0.9915720878122718)</t>
+  </si>
+  <si>
+    <t>('B2a_0g_0', 0.9999909842470821)</t>
+  </si>
+  <si>
+    <t>('lrig_0_cd_0', 0.9999794695745176)</t>
+  </si>
+  <si>
+    <t>('primsev_cocaine', 0.9982901107709041)</t>
+  </si>
+  <si>
+    <t>('primsev_other', 1.0203775297571236)</t>
+  </si>
+  <si>
+    <t>('primsev_alcohol', 1.00009328553864)</t>
+  </si>
+  <si>
+    <t>('female', 0.994057271737192)</t>
+  </si>
+  <si>
+    <t>('dssg_0_cd_0', 0.9580430160133286)</t>
+  </si>
+  <si>
+    <t>('r4ag_0_cd_0', 0.8556426711986002)</t>
+  </si>
+  <si>
+    <t>('%_povertyg_0', 0.9999809545432871)</t>
+  </si>
+  <si>
+    <t>('PYS9Sxg_cd_0', 0.9498168980577506)</t>
+  </si>
+  <si>
+    <t>('epsg_0_cd_0', 0.9774022302859032)</t>
+  </si>
+  <si>
+    <t>('nonwhite', 0.9714536520650838)</t>
+  </si>
+  <si>
+    <t>('primsev_amphetamines', 0.9980408893606477)</t>
+  </si>
+  <si>
+    <t>('SESg_0_cd_0', 0.9712181122033132)</t>
+  </si>
+  <si>
+    <t>('pop_deng_0', 1.0861808210520414)</t>
+  </si>
+  <si>
+    <t>('murder_numg_0', 0.9999316869277205)</t>
+  </si>
+  <si>
+    <t>('primsev_opioids', 1.2105622990579752)</t>
+  </si>
+  <si>
+    <t>('adhdg_0_cd_0', 1.0028924419506895)</t>
+  </si>
+  <si>
+    <t>('gvsg_cd_0', 0.9991795332089884)</t>
+  </si>
+  <si>
+    <t>('prsatx_cd_0', 0.994756177230485)</t>
+  </si>
+  <si>
+    <t>('unemplmt_cd', 0.9994458783679182)</t>
+  </si>
+  <si>
+    <t>('cjsig_0_cd_0', 0.9964874503595882)</t>
+  </si>
+  <si>
+    <t>('srig_0_cd_0', 1.000240458266894)</t>
+  </si>
+  <si>
+    <t>('CWSg_0_cd_0', 0.9999752040520337)</t>
+  </si>
+  <si>
+    <t>('homeless_0_cd_0', 1.000162845822144)</t>
+  </si>
+  <si>
+    <t>('cdsg_0_cd_0', 0.993758628657143)</t>
+  </si>
+  <si>
+    <t>('primsev_marijuana', 0.9999750940128105)</t>
+  </si>
+  <si>
+    <t>('ncar_cd_0', 1.004788331018085)</t>
+  </si>
+  <si>
+    <t>('TRIg_0_cd_0', 1.002325222476289)</t>
   </si>
   <si>
     <t>('B2a_0g_2', 0.8913844065820185)</t>
   </si>
   <si>
-    <t>('pop_deng_0', 1.0861808210520414)</t>
-  </si>
-  <si>
-    <t>('primsev_opioids', 1.2105622990579752)</t>
-  </si>
-  <si>
-    <t>('PYS9Sxg_cd_0', 0.9498168980577506)</t>
+    <t>('lrig_0_cd_2', 1.0000068156418493)</t>
+  </si>
+  <si>
+    <t>('dssg_0_cd_2', 1.0646292988841461)</t>
+  </si>
+  <si>
+    <t>('r4ag_0_cd_2', 0.99987473100723)</t>
+  </si>
+  <si>
+    <t>('PYS9Sxg_cd_2', 1.0023884841404467)</t>
+  </si>
+  <si>
+    <t>('epsg_0_cd_2', 0.9944624041935283)</t>
+  </si>
+  <si>
+    <t>('SESg_0_cd_2', 1.0026608087802165)</t>
+  </si>
+  <si>
+    <t>('pop_deng_2', 1.0004315809631443)</t>
+  </si>
+  <si>
+    <t>('murder_numg_2', 0.9999554947127359)</t>
+  </si>
+  <si>
+    <t>('adhdg_0_cd_2', 1.0291653517774937)</t>
+  </si>
+  <si>
+    <t>('gvsg_cd_2', 0.9999786033938711)</t>
+  </si>
+  <si>
+    <t>('cjsig_0_cd_2', 1.0013913966483587)</t>
   </si>
   <si>
     <t>('srig_0_cd_2', 1.039404288407427)</t>
   </si>
   <si>
-    <t>('cjsig_0_cd_0', 0.0)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_0', 0.9580430160133286)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_0', 0.8556426711986002)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_2', 1.0646292988841461)</t>
+    <t>('CWSg_0_cd_2', 0.9999968851678663)</t>
+  </si>
+  <si>
+    <t>('cdsg_0_cd_2', 1.0440148144567705)</t>
+  </si>
+  <si>
+    <t>('TRIg_0_cd_2', 1.008133526291738)</t>
   </si>
 </sst>
 </file>
@@ -553,7 +871,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -581,13 +899,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1.000465729018531</v>
+        <v>0.9526899734069508</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -601,10 +919,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -615,10 +933,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.7407936901453327</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -632,13 +950,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0.9526899734069508</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -649,10 +967,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.4102832843429358</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -666,10 +984,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.2902027042155237</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -683,13 +1001,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1.301515199519466</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -700,13 +1018,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1.000465729018531</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -717,10 +1035,10 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.2300131371446614</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -737,10 +1055,10 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -751,13 +1069,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>2.83786793770482</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -768,13 +1086,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>1.938707966804583</v>
+        <v>0.2966411868209981</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -785,13 +1103,285 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>1.301515199519466</v>
+        <v>0.7189085332405787</v>
       </c>
       <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>1.312737097408354</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>0.4102832843429358</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>1.938707966804583</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>0.2527876081504934</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>2.83786793770482</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>29</v>
       </c>
-      <c r="E14" t="s">
-        <v>34</v>
+      <c r="C27">
+        <v>0.3499314949605734</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>0.09115513240884035</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>0.7407936901453327</v>
+      </c>
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +1391,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -829,13 +1419,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1.298634548530925</v>
+        <v>0.7834990018639157</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -849,10 +1439,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -866,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -880,13 +1470,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0.7834990018639157</v>
+        <v>0.9935762382114759</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
+        <v>81</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -897,10 +1487,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.9525989106710896</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -914,10 +1504,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0.7606383529901449</v>
+        <v>0.7638073487664213</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -934,10 +1524,10 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -948,13 +1538,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.9935762382114759</v>
+        <v>1.298634548530925</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -965,10 +1555,10 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1.433817979556264</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -982,13 +1572,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1.433817979556264</v>
+        <v>0.3625747111100873</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1002,10 +1592,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1016,13 +1606,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0.6223136826343577</v>
+        <v>0.05791779546572728</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
+        <v>89</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1033,13 +1623,285 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.5466391899207441</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
+        <v>90</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>0.2619849196106233</v>
+      </c>
+      <c r="D15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>0.9525989106710896</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>0.6223136826343577</v>
+      </c>
+      <c r="D17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>0.7606383529901449</v>
+      </c>
+      <c r="D18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>1.1624615877973</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>0.1588701058663767</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>0.5869884222252345</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>0.4597371838867874</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>0.004126920701221839</v>
+      </c>
+      <c r="D24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>0.538002528103438</v>
+      </c>
+      <c r="D26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1049,7 +1911,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1077,13 +1939,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.7595360888429988</v>
+        <v>2.62044775026754</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1094,13 +1956,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.9887906225024075</v>
+        <v>0.1834774982637219</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1111,10 +1973,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.1544149480942987</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1128,13 +1990,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>2.62044775026754</v>
+        <v>0.3867703981203201</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
+        <v>124</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1145,10 +2007,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.6818917604653789</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1162,10 +2024,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.2451632224711889</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1179,13 +2041,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>2.184353466288723</v>
+        <v>0.4093448693900489</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+        <v>127</v>
+      </c>
+      <c r="E8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1196,13 +2058,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.7595360888429988</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1213,10 +2075,10 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0.899707423342836</v>
+        <v>1.190777061096861</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1230,13 +2092,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1.190777061096861</v>
+        <v>2.184353466288723</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
+        <v>130</v>
+      </c>
+      <c r="E11" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1247,13 +2109,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>0.5483146179352071</v>
+        <v>0.01768427526477057</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1264,13 +2126,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.9887906225024075</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
+        <v>132</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1281,13 +2143,285 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.4771235778646361</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" t="s">
-        <v>59</v>
+        <v>133</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>0.6147570447112821</v>
+      </c>
+      <c r="D15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>0.6818917604653789</v>
+      </c>
+      <c r="D16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>0.4563884516825428</v>
+      </c>
+      <c r="D17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>0.4566600730254796</v>
+      </c>
+      <c r="D18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>0.006685921817826019</v>
+      </c>
+      <c r="D19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>0.5354495123518069</v>
+      </c>
+      <c r="D20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>0.08741711242060614</v>
+      </c>
+      <c r="D21" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>0.1991388976997396</v>
+      </c>
+      <c r="D22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>0.5483146179352071</v>
+      </c>
+      <c r="D23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>0.899707423342836</v>
+      </c>
+      <c r="D24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>0.5062158315858265</v>
+      </c>
+      <c r="D25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>0.4459698563356352</v>
+      </c>
+      <c r="D27" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>0.5050947068015957</v>
+      </c>
+      <c r="D29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>0.4731117515681075</v>
+      </c>
+      <c r="D30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E30" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted excel spreadsheet data
</commit_message>
<xml_diff>
--- a/graphs/common_feature_analysis.xlsx
+++ b/graphs/common_feature_analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="172">
   <si>
     <t>Feature</t>
   </si>
@@ -33,6 +33,9 @@
     <t>B2a_0g</t>
   </si>
   <si>
+    <t>%_unemployedg</t>
+  </si>
+  <si>
     <t>lrig_0_cd</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
     <t>%_povertyg</t>
   </si>
   <si>
+    <t>%_public_assistanceg</t>
+  </si>
+  <si>
     <t>PYS9Sxg_cd</t>
   </si>
   <si>
@@ -93,6 +99,9 @@
     <t>unemplmt_cd</t>
   </si>
   <si>
+    <t>%_dropoutg</t>
+  </si>
+  <si>
     <t>cjsig_0_cd</t>
   </si>
   <si>
@@ -120,6 +129,9 @@
     <t>('B2a_0g_0', 0.9412357823218712)</t>
   </si>
   <si>
+    <t>('%_unemployedg_0', 1.0)</t>
+  </si>
+  <si>
     <t>('lrig_0_cd_0', 0.9977892237691484)</t>
   </si>
   <si>
@@ -144,6 +156,9 @@
     <t>('%_povertyg_0', 0.9428459229572359)</t>
   </si>
   <si>
+    <t>('%_public_assistanceg_0', 1.0)</t>
+  </si>
+  <si>
     <t>('PYS9Sxg_cd_0', 0.9879839962248869)</t>
   </si>
   <si>
@@ -159,7 +174,7 @@
     <t>('SESg_0_cd_0', 0.995504554903149)</t>
   </si>
   <si>
-    <t>('pop_deng_0', 0.0)</t>
+    <t>('pop_deng_0', 1.0)</t>
   </si>
   <si>
     <t>('murder_numg_0', 1.4391733054685725)</t>
@@ -180,6 +195,9 @@
     <t>('unemplmt_cd', 0.9922395728915905)</t>
   </si>
   <si>
+    <t>('%_dropoutg_0', 1.0)</t>
+  </si>
+  <si>
     <t>('cjsig_0_cd_0', 0.9208582510771413)</t>
   </si>
   <si>
@@ -216,7 +234,7 @@
     <t>('r4ag_0_cd_2', 1.1779218746872526)</t>
   </si>
   <si>
-    <t>('PYS9Sxg_cd_2', 0.0)</t>
+    <t>('PYS9Sxg_cd_2', 1.0)</t>
   </si>
   <si>
     <t>('epsg_0_cd_2', 0.9999470231363313)</t>
@@ -225,7 +243,7 @@
     <t>('SESg_0_cd_2', 0.9830581368257205)</t>
   </si>
   <si>
-    <t>('pop_deng_2', 0.0)</t>
+    <t>('pop_deng_2', 1.0)</t>
   </si>
   <si>
     <t>('murder_numg_2', 1.003401526386335)</t>
@@ -243,10 +261,10 @@
     <t>('srig_0_cd_2', 0.9998494995714677)</t>
   </si>
   <si>
-    <t>('CWSg_0_cd_2', 0.0)</t>
-  </si>
-  <si>
-    <t>('cdsg_0_cd_2', 0.0)</t>
+    <t>('CWSg_0_cd_2', 1.0)</t>
+  </si>
+  <si>
+    <t>('cdsg_0_cd_2', 1.0)</t>
   </si>
   <si>
     <t>('TRIg_0_cd_2', 0.9878892609049318)</t>
@@ -297,7 +315,7 @@
     <t>('pop_deng_0', 1.0546216678905302)</t>
   </si>
   <si>
-    <t>('murder_numg_0', 0.0)</t>
+    <t>('murder_numg_0', 1.0)</t>
   </si>
   <si>
     <t>('primsev_opioids', 1.001360177902959)</t>
@@ -871,7 +889,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -902,10 +920,10 @@
         <v>0.9526899734069508</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -916,13 +934,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.3641328226092738</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>63</v>
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -936,10 +954,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -953,7 +971,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -970,7 +988,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -984,10 +1002,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0.2902027042155237</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1001,13 +1019,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>1.301515199519466</v>
+        <v>0.2902027042155237</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1018,13 +1036,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>1.000465729018531</v>
+        <v>1.301515199519466</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1035,13 +1053,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0.2300131371446614</v>
+        <v>1.000465729018531</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1052,13 +1070,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.2300131371446614</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>66</v>
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1072,10 +1090,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1086,13 +1104,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0.2966411868209981</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1103,13 +1121,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0.7189085332405787</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1120,13 +1138,13 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>1.312737097408354</v>
+        <v>0.2966411868209981</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
+        <v>49</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1137,13 +1155,13 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.4102832843429358</v>
+        <v>0.7189085332405787</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1154,13 +1172,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>1.938707966804583</v>
+        <v>1.312737097408354</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1171,13 +1189,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.4102832843429358</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1188,13 +1206,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1.938707966804583</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1208,10 +1226,10 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" t="s">
-        <v>72</v>
+        <v>54</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1225,10 +1243,10 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1239,13 +1257,13 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>0.2527876081504934</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1256,13 +1274,13 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>2.83786793770482</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" t="s">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1273,13 +1291,13 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>0.2527876081504934</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" t="s">
-        <v>74</v>
+        <v>58</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1290,13 +1308,13 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>0.3076211386496872</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" t="s">
-        <v>75</v>
+        <v>59</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1307,13 +1325,13 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2.83786793770482</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="E26" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1324,13 +1342,13 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>0.3499314949605734</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1341,13 +1359,13 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>0.09115513240884035</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1358,10 +1376,10 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>0.7407936901453327</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1375,13 +1393,64 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.3499314949605734</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>0.09115513240884035</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>0.7407936901453327</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1391,7 +1460,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1422,10 +1491,10 @@
         <v>0.7834990018639157</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1436,13 +1505,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.4281924686817782</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" t="s">
-        <v>108</v>
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1456,10 +1525,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1470,10 +1539,10 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0.9935762382114759</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1487,10 +1556,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.9935762382114759</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1504,10 +1573,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0.7638073487664213</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1521,13 +1590,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.7638073487664213</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" t="s">
-        <v>109</v>
+        <v>89</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1538,13 +1607,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>1.298634548530925</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1555,13 +1624,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1.433817979556264</v>
+        <v>1.298634548530925</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1572,13 +1641,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0.3625747111100873</v>
+        <v>1.433817979556264</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" t="s">
-        <v>66</v>
+        <v>92</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1592,10 +1661,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" t="s">
-        <v>111</v>
+        <v>46</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1606,13 +1675,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0.05791779546572728</v>
+        <v>0.3625747111100873</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
+        <v>93</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1623,13 +1692,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0.5466391899207441</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="E14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1640,13 +1709,13 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>0.2619849196106233</v>
+        <v>0.05791779546572728</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" t="s">
-        <v>112</v>
+        <v>95</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1657,13 +1726,13 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.9525989106710896</v>
+        <v>0.5466391899207441</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
+        <v>96</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1674,13 +1743,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0.6223136826343577</v>
+        <v>0.2619849196106233</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1691,13 +1760,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.7606383529901449</v>
+        <v>0.9525989106710896</v>
       </c>
       <c r="D18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
+        <v>98</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1708,13 +1777,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.6223136826343577</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1725,13 +1794,13 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>1.1624615877973</v>
+        <v>0.7606383529901449</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" t="s">
-        <v>115</v>
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1742,13 +1811,13 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>0.1588701058663767</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
+        <v>101</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1759,13 +1828,13 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>0.5869884222252345</v>
+        <v>1.1624615877973</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
+        <v>102</v>
+      </c>
+      <c r="E22" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1776,13 +1845,13 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>0.4597371838867874</v>
+        <v>0.1588701058663767</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" t="s">
-        <v>116</v>
+        <v>103</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1793,13 +1862,13 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>0.004126920701221839</v>
+        <v>0.5869884222252345</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" t="s">
-        <v>117</v>
+        <v>104</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1810,13 +1879,13 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>0.1609379062693596</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" t="s">
-        <v>118</v>
+        <v>59</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1827,13 +1896,13 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>0.538002528103438</v>
+        <v>0.4597371838867874</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
+        <v>105</v>
+      </c>
+      <c r="E26" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1844,13 +1913,13 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>0.004126920701221839</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E27" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1864,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="E28" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1878,10 +1947,10 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>0.538002528103438</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1898,10 +1967,61 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E30" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1911,7 +2031,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1942,10 +2062,10 @@
         <v>2.62044775026754</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1956,13 +2076,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.1834774982637219</v>
+        <v>0.4276418954575115</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" t="s">
-        <v>151</v>
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1973,13 +2093,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.1544149480942987</v>
+        <v>0.1834774982637219</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+        <v>128</v>
+      </c>
+      <c r="E4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1990,10 +2110,10 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0.3867703981203201</v>
+        <v>0.1544149480942987</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2007,10 +2127,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.3867703981203201</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2024,10 +2144,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0.2451632224711889</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2041,13 +2161,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0.4093448693900489</v>
+        <v>0.2451632224711889</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" t="s">
-        <v>152</v>
+        <v>132</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2058,13 +2178,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.7595360888429988</v>
+        <v>0.4093448693900489</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2075,13 +2195,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1.190777061096861</v>
+        <v>0.7595360888429988</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
+        <v>134</v>
+      </c>
+      <c r="E10" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2092,13 +2212,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>2.184353466288723</v>
+        <v>1.190777061096861</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" t="s">
-        <v>154</v>
+        <v>135</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2109,13 +2229,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>0.01768427526477057</v>
+        <v>0.2537928859234548</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" t="s">
-        <v>155</v>
+        <v>46</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2126,13 +2246,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0.9887906225024075</v>
+        <v>2.184353466288723</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
+        <v>136</v>
+      </c>
+      <c r="E13" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2143,13 +2263,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0.4771235778646361</v>
+        <v>0.01768427526477057</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
+        <v>137</v>
+      </c>
+      <c r="E14" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2160,13 +2280,13 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>0.6147570447112821</v>
+        <v>0.9887906225024075</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" t="s">
-        <v>156</v>
+        <v>138</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2177,13 +2297,13 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.6818917604653789</v>
+        <v>0.4771235778646361</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" t="s">
-        <v>157</v>
+        <v>139</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2194,13 +2314,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0.4563884516825428</v>
+        <v>0.6147570447112821</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2211,13 +2331,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.4566600730254796</v>
+        <v>0.6818917604653789</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
+        <v>141</v>
+      </c>
+      <c r="E18" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2228,13 +2348,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>0.006685921817826019</v>
+        <v>0.4563884516825428</v>
       </c>
       <c r="D19" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2245,13 +2365,13 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>0.5354495123518069</v>
+        <v>0.4566600730254796</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
-      </c>
-      <c r="E20" t="s">
-        <v>160</v>
+        <v>143</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2262,13 +2382,13 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>0.08741711242060614</v>
+        <v>0.006685921817826019</v>
       </c>
       <c r="D21" t="s">
-        <v>140</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
+        <v>144</v>
+      </c>
+      <c r="E21" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2279,13 +2399,13 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>0.1991388976997396</v>
+        <v>0.5354495123518069</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
+        <v>145</v>
+      </c>
+      <c r="E22" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2296,13 +2416,13 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>0.5483146179352071</v>
+        <v>0.08741711242060614</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E23" t="s">
-        <v>161</v>
+        <v>146</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2313,13 +2433,13 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>0.899707423342836</v>
+        <v>0.1991388976997396</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
-      </c>
-      <c r="E24" t="s">
-        <v>162</v>
+        <v>147</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2330,13 +2450,13 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>0.5062158315858265</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
-      </c>
-      <c r="E25" t="s">
-        <v>163</v>
+        <v>59</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2347,13 +2467,13 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>0.5483146179352071</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
+        <v>148</v>
+      </c>
+      <c r="E26" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2364,13 +2484,13 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>0.4459698563356352</v>
+        <v>0.899707423342836</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E27" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2381,13 +2501,13 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>0.5062158315858265</v>
       </c>
       <c r="D28" t="s">
-        <v>147</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
+        <v>150</v>
+      </c>
+      <c r="E28" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2398,10 +2518,10 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>0.5050947068015957</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -2415,13 +2535,64 @@
         <v>32</v>
       </c>
       <c r="C30">
+        <v>0.4459698563356352</v>
+      </c>
+      <c r="D30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>0.5050947068015957</v>
+      </c>
+      <c r="D32" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33">
         <v>0.4731117515681075</v>
       </c>
-      <c r="D30" t="s">
-        <v>149</v>
-      </c>
-      <c r="E30" t="s">
-        <v>165</v>
+      <c r="D33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lasso uses features RF deems important
</commit_message>
<xml_diff>
--- a/graphs/common_feature_analysis.xlsx
+++ b/graphs/common_feature_analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
   <si>
     <t>Feature</t>
   </si>
@@ -24,514 +24,106 @@
     <t>RF</t>
   </si>
   <si>
-    <t>Lasso</t>
-  </si>
-  <si>
-    <t>Lasso_</t>
+    <t>Lasso_0</t>
+  </si>
+  <si>
+    <t>Lasso_2</t>
+  </si>
+  <si>
+    <t>CWSg_0_cd</t>
+  </si>
+  <si>
+    <t>TRIg_0_cd</t>
+  </si>
+  <si>
+    <t>murder_numg</t>
+  </si>
+  <si>
+    <t>primsev_other</t>
+  </si>
+  <si>
+    <t>PYS9Sxg_cd</t>
+  </si>
+  <si>
+    <t>dssg_0_cd</t>
+  </si>
+  <si>
+    <t>r4ag_0_cd</t>
+  </si>
+  <si>
+    <t>primsev_alcohol</t>
+  </si>
+  <si>
+    <t>%_dropoutg</t>
+  </si>
+  <si>
+    <t>unemplmt_cd</t>
+  </si>
+  <si>
+    <t>pop_deng</t>
+  </si>
+  <si>
+    <t>prsatx_cd</t>
+  </si>
+  <si>
+    <t>cdsg_0_cd</t>
+  </si>
+  <si>
+    <t>nonwhite</t>
+  </si>
+  <si>
+    <t>%_unemployedg</t>
+  </si>
+  <si>
+    <t>gvsg_cd</t>
+  </si>
+  <si>
+    <t>%_public_assistanceg</t>
+  </si>
+  <si>
+    <t>cjsig_0_cd</t>
+  </si>
+  <si>
+    <t>ncar_cd</t>
+  </si>
+  <si>
+    <t>lrig_0_cd</t>
   </si>
   <si>
     <t>B2a_0g</t>
   </si>
   <si>
-    <t>%_unemployedg</t>
-  </si>
-  <si>
-    <t>lrig_0_cd</t>
+    <t>%_povertyg</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>adhdg_0_cd</t>
+  </si>
+  <si>
+    <t>epsg_0_cd</t>
+  </si>
+  <si>
+    <t>primsev_marijuana</t>
+  </si>
+  <si>
+    <t>homeless_0_cd</t>
   </si>
   <si>
     <t>primsev_cocaine</t>
   </si>
   <si>
-    <t>primsev_other</t>
-  </si>
-  <si>
-    <t>primsev_alcohol</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>dssg_0_cd</t>
-  </si>
-  <si>
-    <t>r4ag_0_cd</t>
-  </si>
-  <si>
-    <t>%_povertyg</t>
-  </si>
-  <si>
-    <t>%_public_assistanceg</t>
-  </si>
-  <si>
-    <t>PYS9Sxg_cd</t>
-  </si>
-  <si>
-    <t>epsg_0_cd</t>
-  </si>
-  <si>
-    <t>nonwhite</t>
+    <t>srig_0_cd</t>
+  </si>
+  <si>
+    <t>primsev_opioids</t>
+  </si>
+  <si>
+    <t>SESg_0_cd</t>
   </si>
   <si>
     <t>primsev_amphetamines</t>
-  </si>
-  <si>
-    <t>SESg_0_cd</t>
-  </si>
-  <si>
-    <t>pop_deng</t>
-  </si>
-  <si>
-    <t>murder_numg</t>
-  </si>
-  <si>
-    <t>primsev_opioids</t>
-  </si>
-  <si>
-    <t>adhdg_0_cd</t>
-  </si>
-  <si>
-    <t>gvsg_cd</t>
-  </si>
-  <si>
-    <t>prsatx_cd</t>
-  </si>
-  <si>
-    <t>unemplmt_cd</t>
-  </si>
-  <si>
-    <t>%_dropoutg</t>
-  </si>
-  <si>
-    <t>cjsig_0_cd</t>
-  </si>
-  <si>
-    <t>srig_0_cd</t>
-  </si>
-  <si>
-    <t>CWSg_0_cd</t>
-  </si>
-  <si>
-    <t>homeless_0_cd</t>
-  </si>
-  <si>
-    <t>cdsg_0_cd</t>
-  </si>
-  <si>
-    <t>primsev_marijuana</t>
-  </si>
-  <si>
-    <t>ncar_cd</t>
-  </si>
-  <si>
-    <t>TRIg_0_cd</t>
-  </si>
-  <si>
-    <t>('B2a_0g_0', 0.9412357823218712)</t>
-  </si>
-  <si>
-    <t>('%_unemployedg_0', 1.0)</t>
-  </si>
-  <si>
-    <t>('lrig_0_cd_0', 0.9977892237691484)</t>
-  </si>
-  <si>
-    <t>('primsev_cocaine', 1.0179736684060987)</t>
-  </si>
-  <si>
-    <t>('primsev_other', 1.0014911750546007)</t>
-  </si>
-  <si>
-    <t>('primsev_alcohol', 0.987338482392838)</t>
-  </si>
-  <si>
-    <t>('female', 1.0002922034547932)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_0', 0.9441341914929483)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_0', 0.9946156235050998)</t>
-  </si>
-  <si>
-    <t>('%_povertyg_0', 0.9428459229572359)</t>
-  </si>
-  <si>
-    <t>('%_public_assistanceg_0', 1.0)</t>
-  </si>
-  <si>
-    <t>('PYS9Sxg_cd_0', 0.9879839962248869)</t>
-  </si>
-  <si>
-    <t>('epsg_0_cd_0', 1.007377978538842)</t>
-  </si>
-  <si>
-    <t>('nonwhite', 0.9200349429378138)</t>
-  </si>
-  <si>
-    <t>('primsev_amphetamines', 0.944771776282438)</t>
-  </si>
-  <si>
-    <t>('SESg_0_cd_0', 0.995504554903149)</t>
-  </si>
-  <si>
-    <t>('pop_deng_0', 1.0)</t>
-  </si>
-  <si>
-    <t>('murder_numg_0', 1.4391733054685725)</t>
-  </si>
-  <si>
-    <t>('primsev_opioids', 1.026428458348139)</t>
-  </si>
-  <si>
-    <t>('adhdg_0_cd_0', 0.9994294807189732)</t>
-  </si>
-  <si>
-    <t>('gvsg_cd_0', 0.9566823627609788)</t>
-  </si>
-  <si>
-    <t>('prsatx_cd_0', 1.000255464342523)</t>
-  </si>
-  <si>
-    <t>('unemplmt_cd', 0.9922395728915905)</t>
-  </si>
-  <si>
-    <t>('%_dropoutg_0', 1.0)</t>
-  </si>
-  <si>
-    <t>('cjsig_0_cd_0', 0.9208582510771413)</t>
-  </si>
-  <si>
-    <t>('srig_0_cd_0', 0.9994028046273031)</t>
-  </si>
-  <si>
-    <t>('CWSg_0_cd_0', 0.9992729119011987)</t>
-  </si>
-  <si>
-    <t>('homeless_0_cd_0', 1.003953393254234)</t>
-  </si>
-  <si>
-    <t>('cdsg_0_cd_0', 0.9975251447420269)</t>
-  </si>
-  <si>
-    <t>('primsev_marijuana', 0.9997125598888561)</t>
-  </si>
-  <si>
-    <t>('ncar_cd_0', 1.0682566904441027)</t>
-  </si>
-  <si>
-    <t>('TRIg_0_cd_0', 0.999951925545857)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_2', 1.128348158691236)</t>
-  </si>
-  <si>
-    <t>('lrig_0_cd_2', 0.9973214039209904)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_2', 1.0000551990385265)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_2', 1.1779218746872526)</t>
-  </si>
-  <si>
-    <t>('PYS9Sxg_cd_2', 1.0)</t>
-  </si>
-  <si>
-    <t>('epsg_0_cd_2', 0.9999470231363313)</t>
-  </si>
-  <si>
-    <t>('SESg_0_cd_2', 0.9830581368257205)</t>
-  </si>
-  <si>
-    <t>('pop_deng_2', 1.0)</t>
-  </si>
-  <si>
-    <t>('murder_numg_2', 1.003401526386335)</t>
-  </si>
-  <si>
-    <t>('adhdg_0_cd_2', 1.0052338567367003)</t>
-  </si>
-  <si>
-    <t>('gvsg_cd_2', 1.0041789625594866)</t>
-  </si>
-  <si>
-    <t>('cjsig_0_cd_2', 1.074330210753723)</t>
-  </si>
-  <si>
-    <t>('srig_0_cd_2', 0.9998494995714677)</t>
-  </si>
-  <si>
-    <t>('CWSg_0_cd_2', 1.0)</t>
-  </si>
-  <si>
-    <t>('cdsg_0_cd_2', 1.0)</t>
-  </si>
-  <si>
-    <t>('TRIg_0_cd_2', 0.9878892609049318)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_0', 0.9827316912641159)</t>
-  </si>
-  <si>
-    <t>('lrig_0_cd_0', 0.9772117616051937)</t>
-  </si>
-  <si>
-    <t>('primsev_cocaine', 1.026355968573712)</t>
-  </si>
-  <si>
-    <t>('primsev_other', 1.0497040679188336)</t>
-  </si>
-  <si>
-    <t>('primsev_alcohol', 0.957609263934147)</t>
-  </si>
-  <si>
-    <t>('female', 0.9937523800149287)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_0', 1.000114003069927)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_0', 0.8946958002258929)</t>
-  </si>
-  <si>
-    <t>('%_povertyg_0', 0.9739665008654048)</t>
-  </si>
-  <si>
-    <t>('PYS9Sxg_cd_0', 0.9353836116963504)</t>
-  </si>
-  <si>
-    <t>('epsg_0_cd_0', 0.9969418452634656)</t>
-  </si>
-  <si>
-    <t>('nonwhite', 0.9189422138816976)</t>
-  </si>
-  <si>
-    <t>('primsev_amphetamines', 0.9838176681964953)</t>
-  </si>
-  <si>
-    <t>('SESg_0_cd_0', 0.997424526647715)</t>
-  </si>
-  <si>
-    <t>('pop_deng_0', 1.0546216678905302)</t>
-  </si>
-  <si>
-    <t>('murder_numg_0', 1.0)</t>
-  </si>
-  <si>
-    <t>('primsev_opioids', 1.001360177902959)</t>
-  </si>
-  <si>
-    <t>('adhdg_0_cd_0', 1.0001743918236392)</t>
-  </si>
-  <si>
-    <t>('gvsg_cd_0', 0.9952267711981352)</t>
-  </si>
-  <si>
-    <t>('prsatx_cd_0', 0.9411367306303198)</t>
-  </si>
-  <si>
-    <t>('unemplmt_cd', 0.9952859575926934)</t>
-  </si>
-  <si>
-    <t>('cjsig_0_cd_0', 0.9354206641997593)</t>
-  </si>
-  <si>
-    <t>('srig_0_cd_0', 0.9985401922503998)</t>
-  </si>
-  <si>
-    <t>('CWSg_0_cd_0', 1.0041140618481026)</t>
-  </si>
-  <si>
-    <t>('homeless_0_cd_0', 1.0021357370718738)</t>
-  </si>
-  <si>
-    <t>('cdsg_0_cd_0', 0.9468888416799393)</t>
-  </si>
-  <si>
-    <t>('primsev_marijuana', 0.9998460155514156)</t>
-  </si>
-  <si>
-    <t>('ncar_cd_0', 1.0074496367042836)</t>
-  </si>
-  <si>
-    <t>('TRIg_0_cd_0', 1.0242608134558155)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_2', 0.9763382997222922)</t>
-  </si>
-  <si>
-    <t>('lrig_0_cd_2', 1.0030057032567987)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_2', 0.9876473847842663)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_2', 0.9974870090150953)</t>
-  </si>
-  <si>
-    <t>('epsg_0_cd_2', 1.0423813392017787)</t>
-  </si>
-  <si>
-    <t>('SESg_0_cd_2', 0.9897939071604813)</t>
-  </si>
-  <si>
-    <t>('murder_numg_2', 0.9575506176558319)</t>
-  </si>
-  <si>
-    <t>('adhdg_0_cd_2', 0.9997572102938117)</t>
-  </si>
-  <si>
-    <t>('gvsg_cd_2', 0.9910236335438817)</t>
-  </si>
-  <si>
-    <t>('cjsig_0_cd_2', 0.9986804452510393)</t>
-  </si>
-  <si>
-    <t>('srig_0_cd_2', 1.0183149928931163)</t>
-  </si>
-  <si>
-    <t>('CWSg_0_cd_2', 1.0025903321333538)</t>
-  </si>
-  <si>
-    <t>('cdsg_0_cd_2', 0.9999997889576135)</t>
-  </si>
-  <si>
-    <t>('TRIg_0_cd_2', 0.9915720878122718)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_0', 0.9999909842470821)</t>
-  </si>
-  <si>
-    <t>('lrig_0_cd_0', 0.9999794695745176)</t>
-  </si>
-  <si>
-    <t>('primsev_cocaine', 0.9982901107709041)</t>
-  </si>
-  <si>
-    <t>('primsev_other', 1.0203775297571236)</t>
-  </si>
-  <si>
-    <t>('primsev_alcohol', 1.00009328553864)</t>
-  </si>
-  <si>
-    <t>('female', 0.994057271737192)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_0', 0.9580430160133286)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_0', 0.8556426711986002)</t>
-  </si>
-  <si>
-    <t>('%_povertyg_0', 0.9999809545432871)</t>
-  </si>
-  <si>
-    <t>('PYS9Sxg_cd_0', 0.9498168980577506)</t>
-  </si>
-  <si>
-    <t>('epsg_0_cd_0', 0.9774022302859032)</t>
-  </si>
-  <si>
-    <t>('nonwhite', 0.9714536520650838)</t>
-  </si>
-  <si>
-    <t>('primsev_amphetamines', 0.9980408893606477)</t>
-  </si>
-  <si>
-    <t>('SESg_0_cd_0', 0.9712181122033132)</t>
-  </si>
-  <si>
-    <t>('pop_deng_0', 1.0861808210520414)</t>
-  </si>
-  <si>
-    <t>('murder_numg_0', 0.9999316869277205)</t>
-  </si>
-  <si>
-    <t>('primsev_opioids', 1.2105622990579752)</t>
-  </si>
-  <si>
-    <t>('adhdg_0_cd_0', 1.0028924419506895)</t>
-  </si>
-  <si>
-    <t>('gvsg_cd_0', 0.9991795332089884)</t>
-  </si>
-  <si>
-    <t>('prsatx_cd_0', 0.994756177230485)</t>
-  </si>
-  <si>
-    <t>('unemplmt_cd', 0.9994458783679182)</t>
-  </si>
-  <si>
-    <t>('cjsig_0_cd_0', 0.9964874503595882)</t>
-  </si>
-  <si>
-    <t>('srig_0_cd_0', 1.000240458266894)</t>
-  </si>
-  <si>
-    <t>('CWSg_0_cd_0', 0.9999752040520337)</t>
-  </si>
-  <si>
-    <t>('homeless_0_cd_0', 1.000162845822144)</t>
-  </si>
-  <si>
-    <t>('cdsg_0_cd_0', 0.993758628657143)</t>
-  </si>
-  <si>
-    <t>('primsev_marijuana', 0.9999750940128105)</t>
-  </si>
-  <si>
-    <t>('ncar_cd_0', 1.004788331018085)</t>
-  </si>
-  <si>
-    <t>('TRIg_0_cd_0', 1.002325222476289)</t>
-  </si>
-  <si>
-    <t>('B2a_0g_2', 0.8913844065820185)</t>
-  </si>
-  <si>
-    <t>('lrig_0_cd_2', 1.0000068156418493)</t>
-  </si>
-  <si>
-    <t>('dssg_0_cd_2', 1.0646292988841461)</t>
-  </si>
-  <si>
-    <t>('r4ag_0_cd_2', 0.99987473100723)</t>
-  </si>
-  <si>
-    <t>('PYS9Sxg_cd_2', 1.0023884841404467)</t>
-  </si>
-  <si>
-    <t>('epsg_0_cd_2', 0.9944624041935283)</t>
-  </si>
-  <si>
-    <t>('SESg_0_cd_2', 1.0026608087802165)</t>
-  </si>
-  <si>
-    <t>('pop_deng_2', 1.0004315809631443)</t>
-  </si>
-  <si>
-    <t>('murder_numg_2', 0.9999554947127359)</t>
-  </si>
-  <si>
-    <t>('adhdg_0_cd_2', 1.0291653517774937)</t>
-  </si>
-  <si>
-    <t>('gvsg_cd_2', 0.9999786033938711)</t>
-  </si>
-  <si>
-    <t>('cjsig_0_cd_2', 1.0013913966483587)</t>
-  </si>
-  <si>
-    <t>('srig_0_cd_2', 1.039404288407427)</t>
-  </si>
-  <si>
-    <t>('CWSg_0_cd_2', 0.9999968851678663)</t>
-  </si>
-  <si>
-    <t>('cdsg_0_cd_2', 1.0440148144567705)</t>
-  </si>
-  <si>
-    <t>('TRIg_0_cd_2', 1.008133526291738)</t>
   </si>
 </sst>
 </file>
@@ -917,13 +509,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.9526899734069508</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
+        <v>0.7499691323298542</v>
+      </c>
+      <c r="D2">
+        <v>0.999297816883523</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -934,13 +526,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.3641328226092738</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
+        <v>0.6194170589263445</v>
+      </c>
+      <c r="D3">
+        <v>0.999988392693833</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.9886586554110777</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -951,13 +543,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
+        <v>2.246631127131743</v>
+      </c>
+      <c r="D4">
+        <v>1.438177354212656</v>
+      </c>
+      <c r="E4">
+        <v>1.003275508605973</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -970,8 +562,8 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>39</v>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -985,13 +577,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
+        <v>0.826523640076651</v>
+      </c>
+      <c r="D6">
+        <v>0.988112673190045</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1002,13 +594,13 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
+        <v>1.096860236992394</v>
+      </c>
+      <c r="D7">
+        <v>0.9452978887362431</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1.000380152537883</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1019,13 +611,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0.2902027042155237</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
+        <v>1.901716215248086</v>
+      </c>
+      <c r="D8">
+        <v>0.9946272410057734</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1.177694720912766</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1036,13 +628,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>1.301515199519466</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>70</v>
+        <v>0.05478427136436621</v>
+      </c>
+      <c r="D9">
+        <v>0.9875354121731758</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1053,13 +645,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1.000465729018531</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>71</v>
+        <v>0.6197897557156943</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1070,10 +662,10 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0.2300131371446614</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
+        <v>0.3478046822796251</v>
+      </c>
+      <c r="D11">
+        <v>0.9922873914146035</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1087,13 +679,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
+        <v>0.5343963409929628</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1104,13 +696,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
+        <v>1.377382597985057</v>
+      </c>
+      <c r="D13">
+        <v>1.000169717109992</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1123,11 +715,11 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>73</v>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1138,10 +730,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>0.2966411868209981</v>
-      </c>
-      <c r="D15" t="s">
-        <v>49</v>
+        <v>0.9305998850169062</v>
+      </c>
+      <c r="D15">
+        <v>0.9202928292931093</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1155,10 +747,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.7189085332405787</v>
-      </c>
-      <c r="D16" t="s">
-        <v>50</v>
+        <v>0.6938754887300876</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1172,13 +764,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>1.312737097408354</v>
-      </c>
-      <c r="D17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" t="s">
-        <v>74</v>
+        <v>0.002996747377884067</v>
+      </c>
+      <c r="D17">
+        <v>0.9572374070031288</v>
+      </c>
+      <c r="E17">
+        <v>1.004380292684338</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1189,13 +781,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.4102832843429358</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" t="s">
-        <v>75</v>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1206,13 +798,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>1.938707966804583</v>
-      </c>
-      <c r="D19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" t="s">
-        <v>76</v>
+        <v>2.85875029045165</v>
+      </c>
+      <c r="D19">
+        <v>0.9208365826604124</v>
+      </c>
+      <c r="E19">
+        <v>1.074476545643171</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1223,10 +815,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
+        <v>0.7815447441652249</v>
+      </c>
+      <c r="D20">
+        <v>1.068477075485512</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1240,13 +832,13 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" t="s">
-        <v>77</v>
+        <v>0.1146212434663457</v>
+      </c>
+      <c r="D21">
+        <v>0.9978487052693242</v>
+      </c>
+      <c r="E21">
+        <v>0.9970791862061565</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1257,13 +849,13 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" t="s">
-        <v>78</v>
+        <v>1.596035499383908</v>
+      </c>
+      <c r="D22">
+        <v>0.9416126695423144</v>
+      </c>
+      <c r="E22">
+        <v>1.127700813990828</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1274,10 +866,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>57</v>
+        <v>1.735566198725087</v>
+      </c>
+      <c r="D23">
+        <v>0.9428493908275736</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1291,10 +883,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>0.2527876081504934</v>
-      </c>
-      <c r="D24" t="s">
-        <v>58</v>
+        <v>0.4795580471881119</v>
+      </c>
+      <c r="D24">
+        <v>1.000048554786843</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1308,10 +900,10 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>0.3076211386496872</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1325,13 +917,13 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>2.83786793770482</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" t="s">
-        <v>79</v>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1344,11 +936,11 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" t="s">
-        <v>80</v>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1359,13 +951,13 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" t="s">
-        <v>81</v>
+        <v>0.3858805991738878</v>
+      </c>
+      <c r="D28">
+        <v>1.00392973722696</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1376,10 +968,10 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>63</v>
+        <v>0.170742232520319</v>
+      </c>
+      <c r="D29">
+        <v>1.01754716598419</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1393,13 +985,13 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>0.3499314949605734</v>
-      </c>
-      <c r="D30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" t="s">
-        <v>82</v>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1410,10 +1002,10 @@
         <v>33</v>
       </c>
       <c r="C31">
-        <v>0.09115513240884035</v>
-      </c>
-      <c r="D31" t="s">
-        <v>65</v>
+        <v>0.1740902849715134</v>
+      </c>
+      <c r="D31">
+        <v>1.024385633270297</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1427,13 +1019,13 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>0.7407936901453327</v>
-      </c>
-      <c r="D32" t="s">
-        <v>66</v>
+        <v>1.028593017556547</v>
+      </c>
+      <c r="D32">
+        <v>0.9954427898330137</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.9832657707744273</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1444,13 +1036,13 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" t="s">
-        <v>83</v>
+        <v>0.2408577993230447</v>
+      </c>
+      <c r="D33">
+        <v>0.9451473306892698</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1488,13 +1080,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.7834990018639157</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>113</v>
+        <v>0.4430732138363117</v>
+      </c>
+      <c r="D2">
+        <v>1.006646915444035</v>
+      </c>
+      <c r="E2">
+        <v>1.002640861588879</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1505,13 +1097,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.4281924686817782</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
+        <v>0.3200292221140292</v>
+      </c>
+      <c r="D3">
+        <v>1.023334283181696</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.9904482379113281</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1522,13 +1114,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" t="s">
-        <v>114</v>
+        <v>0.522153898212369</v>
+      </c>
+      <c r="D4">
+        <v>1.000272543951826</v>
+      </c>
+      <c r="E4">
+        <v>0.9527251041505546</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1539,10 +1131,10 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>86</v>
+        <v>0.8647357222101946</v>
+      </c>
+      <c r="D5">
+        <v>1.054099624904234</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1556,13 +1148,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.9935762382114759</v>
-      </c>
-      <c r="D6" t="s">
-        <v>87</v>
+        <v>1.374220802745047</v>
+      </c>
+      <c r="D6">
+        <v>0.9210925808114688</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1.000248329911898</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1573,13 +1165,13 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>88</v>
+        <v>0.5694619159304957</v>
+      </c>
+      <c r="D7">
+        <v>1.000182776314048</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.9867452888811322</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1590,13 +1182,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0.7638073487664213</v>
-      </c>
-      <c r="D8" t="s">
-        <v>89</v>
+        <v>1.629504148575506</v>
+      </c>
+      <c r="D8">
+        <v>0.8866226963844589</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.9989302832952005</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1607,13 +1199,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" t="s">
-        <v>115</v>
+        <v>0.1586067047068076</v>
+      </c>
+      <c r="D9">
+        <v>0.9564765334809986</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1624,13 +1216,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1.298634548530925</v>
-      </c>
-      <c r="D10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" t="s">
-        <v>116</v>
+        <v>1.074325565607227</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1641,10 +1233,10 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1.433817979556264</v>
-      </c>
-      <c r="D11" t="s">
-        <v>92</v>
+        <v>0.7588063578091814</v>
+      </c>
+      <c r="D11">
+        <v>0.9932112003921881</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1658,13 +1250,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
+        <v>0.8637555773102719</v>
+      </c>
+      <c r="D12">
+        <v>1.059833145890112</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1675,13 +1267,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0.3625747111100873</v>
-      </c>
-      <c r="D13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
+        <v>1.67842476514416</v>
+      </c>
+      <c r="D13">
+        <v>0.9399928244024633</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1692,13 +1284,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" t="s">
-        <v>117</v>
+        <v>0.03815148543513448</v>
+      </c>
+      <c r="D14">
+        <v>0.9485676168661241</v>
+      </c>
+      <c r="E14">
+        <v>0.9999607113022787</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1709,10 +1301,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>0.05791779546572728</v>
-      </c>
-      <c r="D15" t="s">
-        <v>95</v>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1726,10 +1318,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.5466391899207441</v>
-      </c>
-      <c r="D16" t="s">
-        <v>96</v>
+        <v>0.3724669641848554</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1743,13 +1335,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0.2619849196106233</v>
-      </c>
-      <c r="D17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" t="s">
-        <v>118</v>
+        <v>1.234685045860917</v>
+      </c>
+      <c r="D17">
+        <v>0.9956267734771</v>
+      </c>
+      <c r="E17">
+        <v>0.9894712075281712</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1760,13 +1352,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.9525989106710896</v>
-      </c>
-      <c r="D18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" t="s">
-        <v>75</v>
+        <v>0.0705856063228005</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1777,13 +1369,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>0.6223136826343577</v>
-      </c>
-      <c r="D19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" t="s">
-        <v>119</v>
+        <v>1.524907927206517</v>
+      </c>
+      <c r="D19">
+        <v>0.9406072447346979</v>
+      </c>
+      <c r="E19">
+        <v>0.9973503871207171</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1794,10 +1386,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>0.7606383529901449</v>
-      </c>
-      <c r="D20" t="s">
-        <v>100</v>
+        <v>1.368808291403192</v>
+      </c>
+      <c r="D20">
+        <v>1.010581187645107</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1811,13 +1403,13 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" t="s">
-        <v>120</v>
+        <v>1.104174281170197</v>
+      </c>
+      <c r="D21">
+        <v>0.9774349485611151</v>
+      </c>
+      <c r="E21">
+        <v>1.002991296703505</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1828,13 +1420,13 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>1.1624615877973</v>
-      </c>
-      <c r="D22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" t="s">
-        <v>121</v>
+        <v>0.5950325046255995</v>
+      </c>
+      <c r="D22">
+        <v>0.9803546922488365</v>
+      </c>
+      <c r="E22">
+        <v>0.9768372948180961</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1845,10 +1437,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>0.1588701058663767</v>
-      </c>
-      <c r="D23" t="s">
-        <v>103</v>
+        <v>1.651587743533147</v>
+      </c>
+      <c r="D23">
+        <v>0.985239244796496</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1862,10 +1454,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>0.5869884222252345</v>
-      </c>
-      <c r="D24" t="s">
-        <v>104</v>
+        <v>1.590524098370643</v>
+      </c>
+      <c r="D24">
+        <v>0.9946885105573861</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1879,13 +1471,13 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>0.1609379062693596</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
+        <v>0.7167878135779698</v>
+      </c>
+      <c r="D25">
+        <v>1.000001292721292</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.9999988074316349</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1896,13 +1488,13 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>0.4597371838867874</v>
-      </c>
-      <c r="D26" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" t="s">
-        <v>122</v>
+        <v>0.8954590765187124</v>
+      </c>
+      <c r="D26">
+        <v>0.9944994897927067</v>
+      </c>
+      <c r="E26">
+        <v>1.042957291938359</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1913,13 +1505,13 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>0.004126920701221839</v>
-      </c>
-      <c r="D27" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" t="s">
-        <v>123</v>
+        <v>1.074100390266186</v>
+      </c>
+      <c r="D27">
+        <v>0.9995897274783414</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1930,13 +1522,13 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" t="s">
-        <v>124</v>
+        <v>1.736393130353541</v>
+      </c>
+      <c r="D28">
+        <v>1.00186322608544</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1947,10 +1539,10 @@
         <v>31</v>
       </c>
       <c r="C29">
-        <v>0.538002528103438</v>
-      </c>
-      <c r="D29" t="s">
-        <v>108</v>
+        <v>0.06590929155687544</v>
+      </c>
+      <c r="D29">
+        <v>1.023284194794133</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1964,13 +1556,13 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" t="s">
-        <v>125</v>
+        <v>0.6293172789737191</v>
+      </c>
+      <c r="D30">
+        <v>0.9983393953224563</v>
+      </c>
+      <c r="E30">
+        <v>1.017693097610397</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1981,10 +1573,10 @@
         <v>33</v>
       </c>
       <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31" t="s">
-        <v>110</v>
+        <v>0.3990097410362928</v>
+      </c>
+      <c r="D31">
+        <v>1.003527401873206</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1998,13 +1590,13 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32" t="s">
-        <v>111</v>
+        <v>0.689147632228105</v>
+      </c>
+      <c r="D32">
+        <v>0.9976595871180031</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.9888855409292369</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2015,13 +1607,13 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" t="s">
-        <v>126</v>
+        <v>0.8806627958123061</v>
+      </c>
+      <c r="D33">
+        <v>0.9809873004199945</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2059,13 +1651,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>2.62044775026754</v>
-      </c>
-      <c r="D2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" t="s">
-        <v>156</v>
+        <v>0.6969461460256638</v>
+      </c>
+      <c r="D2">
+        <v>1.00001185924153</v>
+      </c>
+      <c r="E2">
+        <v>1.00026726322185</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2076,13 +1668,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.4276418954575115</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
+        <v>0.5090588059497364</v>
+      </c>
+      <c r="D3">
+        <v>1.001949449463804</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1.010795608513704</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2093,13 +1685,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.1834774982637219</v>
-      </c>
-      <c r="D4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" t="s">
-        <v>157</v>
+        <v>0.320490566430261</v>
+      </c>
+      <c r="D4">
+        <v>0.9999252414216155</v>
+      </c>
+      <c r="E4">
+        <v>0.9998341963257054</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2110,10 +1702,10 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0.1544149480942987</v>
-      </c>
-      <c r="D5" t="s">
-        <v>129</v>
+        <v>0.4450960743994137</v>
+      </c>
+      <c r="D5">
+        <v>1.005522689720825</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2127,13 +1719,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.3867703981203201</v>
-      </c>
-      <c r="D6" t="s">
-        <v>130</v>
+        <v>2.64646913214611</v>
+      </c>
+      <c r="D6">
+        <v>0.93203750434516</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1.035687568346879</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2144,13 +1736,13 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>131</v>
+        <v>0.7343833025457651</v>
+      </c>
+      <c r="D7">
+        <v>0.9518460050944164</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1.069513364216004</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2161,13 +1753,13 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0.2451632224711889</v>
-      </c>
-      <c r="D8" t="s">
-        <v>132</v>
+        <v>1.619575604858416</v>
+      </c>
+      <c r="D8">
+        <v>0.8495889601573247</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1.002926747913522</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2178,13 +1770,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.4093448693900489</v>
-      </c>
-      <c r="D9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E9" t="s">
-        <v>158</v>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2195,13 +1787,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0.7595360888429988</v>
-      </c>
-      <c r="D10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" t="s">
-        <v>159</v>
+        <v>0.2713144327589878</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2212,10 +1804,10 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1.190777061096861</v>
-      </c>
-      <c r="D11" t="s">
-        <v>135</v>
+        <v>0.7185025546978761</v>
+      </c>
+      <c r="D11">
+        <v>0.9999989614365479</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2229,13 +1821,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>0.2537928859234548</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
+        <v>0.7698498397757051</v>
+      </c>
+      <c r="D12">
+        <v>1.080495748433123</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1.000164928537506</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2246,13 +1838,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>2.184353466288723</v>
-      </c>
-      <c r="D13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" t="s">
-        <v>160</v>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2263,13 +1855,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0.01768427526477057</v>
-      </c>
-      <c r="D14" t="s">
-        <v>137</v>
-      </c>
-      <c r="E14" t="s">
-        <v>161</v>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2280,10 +1872,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>0.9887906225024075</v>
-      </c>
-      <c r="D15" t="s">
-        <v>138</v>
+        <v>0.7814728108862459</v>
+      </c>
+      <c r="D15">
+        <v>0.957934035764645</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2297,10 +1889,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.4771235778646361</v>
-      </c>
-      <c r="D16" t="s">
-        <v>139</v>
+        <v>0.3079696364653831</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2314,13 +1906,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0.6147570447112821</v>
-      </c>
-      <c r="D17" t="s">
-        <v>140</v>
-      </c>
-      <c r="E17" t="s">
-        <v>162</v>
+        <v>0.6507894555890871</v>
+      </c>
+      <c r="D17">
+        <v>0.9979390985004893</v>
+      </c>
+      <c r="E17">
+        <v>0.999937880007687</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2331,13 +1923,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.6818917604653789</v>
-      </c>
-      <c r="D18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E18" t="s">
-        <v>163</v>
+        <v>0.2578701181016719</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2348,13 +1940,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>0.4563884516825428</v>
-      </c>
-      <c r="D19" t="s">
-        <v>142</v>
-      </c>
-      <c r="E19" t="s">
-        <v>164</v>
+        <v>0.2462371060274215</v>
+      </c>
+      <c r="D19">
+        <v>0.9960743816987617</v>
+      </c>
+      <c r="E19">
+        <v>1.002055253510075</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2365,10 +1957,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>0.4566600730254796</v>
-      </c>
-      <c r="D20" t="s">
-        <v>143</v>
+        <v>0.7420813984046515</v>
+      </c>
+      <c r="D20">
+        <v>1.010304278202071</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2382,13 +1974,13 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>0.006685921817826019</v>
-      </c>
-      <c r="D21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" t="s">
-        <v>165</v>
+        <v>0.8031314970832772</v>
+      </c>
+      <c r="D21">
+        <v>0.9998578244974077</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2399,13 +1991,13 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>0.5354495123518069</v>
-      </c>
-      <c r="D22" t="s">
-        <v>145</v>
-      </c>
-      <c r="E22" t="s">
-        <v>166</v>
+        <v>2.285924216710981</v>
+      </c>
+      <c r="D22">
+        <v>1.000129859360991</v>
+      </c>
+      <c r="E22">
+        <v>0.9065535520916694</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2416,10 +2008,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>0.08741711242060614</v>
-      </c>
-      <c r="D23" t="s">
-        <v>146</v>
+        <v>0.9523188176159756</v>
+      </c>
+      <c r="D23">
+        <v>0.999905520300827</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2433,10 +2025,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>0.1991388976997396</v>
-      </c>
-      <c r="D24" t="s">
-        <v>147</v>
+        <v>0.1067584388505549</v>
+      </c>
+      <c r="D24">
+        <v>0.9905469772917903</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2450,13 +2042,13 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
+        <v>0.4547550124447584</v>
+      </c>
+      <c r="D25">
+        <v>1.00069017054004</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1.039266008494395</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2467,13 +2059,13 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>0.5483146179352071</v>
-      </c>
-      <c r="D26" t="s">
-        <v>148</v>
-      </c>
-      <c r="E26" t="s">
-        <v>167</v>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2484,13 +2076,13 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>0.899707423342836</v>
-      </c>
-      <c r="D27" t="s">
-        <v>149</v>
-      </c>
-      <c r="E27" t="s">
-        <v>168</v>
+        <v>0.09496790875907629</v>
+      </c>
+      <c r="D27">
+        <v>0.9838875771361666</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2501,13 +2093,13 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>0.5062158315858265</v>
-      </c>
-      <c r="D28" t="s">
-        <v>150</v>
-      </c>
-      <c r="E28" t="s">
-        <v>169</v>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2520,8 +2112,8 @@
       <c r="C29">
         <v>0</v>
       </c>
-      <c r="D29" t="s">
-        <v>151</v>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -2535,13 +2127,13 @@
         <v>32</v>
       </c>
       <c r="C30">
-        <v>0.4459698563356352</v>
-      </c>
-      <c r="D30" t="s">
-        <v>152</v>
-      </c>
-      <c r="E30" t="s">
-        <v>170</v>
+        <v>0.5759609087659625</v>
+      </c>
+      <c r="D30">
+        <v>1.00002962651549</v>
+      </c>
+      <c r="E30">
+        <v>1.036062045589232</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2554,8 +2146,8 @@
       <c r="C31">
         <v>0</v>
       </c>
-      <c r="D31" t="s">
-        <v>153</v>
+      <c r="D31">
+        <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -2569,13 +2161,13 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>0.5050947068015957</v>
-      </c>
-      <c r="D32" t="s">
-        <v>154</v>
+        <v>0.7490988005021804</v>
+      </c>
+      <c r="D32">
+        <v>0.9643772632379808</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1.00299911577903</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2586,13 +2178,13 @@
         <v>35</v>
       </c>
       <c r="C33">
-        <v>0.4731117515681075</v>
-      </c>
-      <c r="D33" t="s">
-        <v>155</v>
-      </c>
-      <c r="E33" t="s">
-        <v>171</v>
+        <v>0.04976362890380404</v>
+      </c>
+      <c r="D33">
+        <v>0.9736092129061202</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>